<commit_message>
Add and update files via upload
Added to supplement Appendix materials during peer review.
</commit_message>
<xml_diff>
--- a/LLMsForDeductiveCoding_Appendix.xlsx
+++ b/LLMsForDeductiveCoding_Appendix.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28619"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C99539E4-63B4-4F7B-A266-1800FE4C3DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshl\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64098AE-383F-44EA-91E2-22A42FD43E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DT Dimensions" sheetId="2" r:id="rId1"/>
@@ -32,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Digital Twin Dimensions (adapted from Jones et al., 2020)</t>
   </si>
@@ -200,12 +205,66 @@
   <si>
     <t>Zhou, S.-W., Guo, S.-S., Xu, W.-X., Du, B.-G., Liang, J.-Y., Wang, L., &amp; Li, Y.-B. (2024). Digital Twin-Based Pump Station Dynamic Scheduling for Energy-Saving Optimization in Water Supply System. Water Resources Management, 38(8), 2773–2789. https://doi.org/10.1007/s11269-024-03791-2</t>
   </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>This project developed a digital twin of a water treatment facility.</t>
+  </si>
+  <si>
+    <t>A digital twin was developed as a virtual replica of the system.</t>
+  </si>
+  <si>
+    <t>This leverages mechanistic models with integrated artificial intelligence.</t>
+  </si>
+  <si>
+    <t>Across the hilly terrain, a population of 50,000 people in a warm climate rely on the physical system.</t>
+  </si>
+  <si>
+    <t>Data is stored in a GIS database to enable modeling. The results from the modeling environment are presented in a visualization application for analysis and utilization.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As the physical system changes, the virtual entity responds by changing its parameters to match those measured. As the digital twin identified operational improvements, it updates the recommended setpoints of valves to achieve that improvement. </t>
+  </si>
+  <si>
+    <t>The output of the digital twin shows good agreement between the digital twin predicted and measured values.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To gather data, in-line flow and temperature sensors track behavior over time. </t>
+  </si>
+  <si>
+    <t>The predicted behavior from the digital twin shows within +/- 5% deviation from the measured values at all times. To account for change over time, the model is continuously calibarated as new data arrives.</t>
+  </si>
+  <si>
+    <t>The model tracks power consumption, fluid pressure, and temperature using estimated efficiency values.</t>
+  </si>
+  <si>
+    <t>The digital twin modeling is updated on 5 minute intervals.</t>
+  </si>
+  <si>
+    <t>The digital twin supports operational efficiency efforts by providing forecasting and optimization.</t>
+  </si>
+  <si>
+    <t>The digital twin will improve production rate while decreasing costs of operation.</t>
+  </si>
+  <si>
+    <t>Data is stored in a secured cloud server. Data is shared via encrypted wireless sensor network which is wholly owned by the utility.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The digital twin mirrors the behavior of the entire system, both within the fence and outside. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The results from the digital twin are then shared with operators who have final say in the execution of the provided suggestions. Other parameters are executed directly through interfacing with actuators in the field. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The digital twin utilizes sensor reading through a wireless sensor network which is passed through SCADA before reaching the digital twin. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,14 +275,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -237,7 +296,7 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -245,7 +304,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -278,21 +337,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -318,19 +368,16 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
@@ -340,13 +387,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9981"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -712,200 +769,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA86F43-79EA-4DC1-ACA9-F0DFBDED2A1A}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="59.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="2" max="2" width="59.88671875" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="45.75">
-      <c r="A3" s="4" t="s">
+      <c r="C2" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="60.75">
-      <c r="A4" s="4" t="s">
+      <c r="C3" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="76.5">
-      <c r="A5" s="4" t="s">
+      <c r="C4" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="45.75">
-      <c r="A6" s="4" t="s">
+      <c r="C5" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="45.75">
-      <c r="A7" s="4" t="s">
+      <c r="C6" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="45.75">
-      <c r="A8" s="4" t="s">
+      <c r="C7" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="30.75">
-      <c r="A9" s="4" t="s">
+      <c r="C8" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="76.5">
-      <c r="A10" s="4" t="s">
+      <c r="C9" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="76.5">
-      <c r="A11" s="4" t="s">
+      <c r="C10" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="388.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="106.5">
-      <c r="A12" s="4" t="s">
+      <c r="C11" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="45.75">
-      <c r="A13" s="4" t="s">
+      <c r="C12" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="30.75">
-      <c r="A14" s="4" t="s">
+      <c r="C13" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="45.75">
-      <c r="A15" s="4" t="s">
+      <c r="C14" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="30.75">
-      <c r="A16" s="4" t="s">
+      <c r="C15" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="45.75">
-      <c r="A17" s="4" t="s">
+      <c r="C16" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="91.5">
-      <c r="A18" s="4" t="s">
+      <c r="C17" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="388.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="45.75">
-      <c r="A19" s="4" t="s">
+      <c r="C18" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="6" t="s">
+      <c r="C19" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A10:B10 A16:B17 A13:B13">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Classification Needed">
-      <formula>NOT(ISERROR(SEARCH("Classification Needed",A10)))</formula>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Classification Needed">
+      <formula>NOT(ISERROR(SEARCH("Classification Needed",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Not discussed">
+      <formula>NOT(ISERROR(SEARCH("Not discussed",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:B19">
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="Not discussed">
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="Classification Needed">
+      <formula>NOT(ISERROR(SEARCH("Classification Needed",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="Not discussed">
       <formula>NOT(ISERROR(SEARCH("Not discussed",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:B9 A11:B15 A18:B19">
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Classification Needed">
-      <formula>NOT(ISERROR(SEARCH("Classification Needed",A2)))</formula>
+  <conditionalFormatting sqref="C2:C19">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Classification Needed">
+      <formula>NOT(ISERROR(SEARCH("Classification Needed",C2)))</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Not discussed">
-      <formula>NOT(ISERROR(SEARCH("Not discussed",A1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Classification Needed">
-      <formula>NOT(ISERROR(SEARCH("Classification Needed",A1)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Not discussed">
+      <formula>NOT(ISERROR(SEARCH("Not discussed",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -923,58 +1035,58 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="57.75">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="101.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="115.5">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="72.75">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="101.25">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="115.5">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="72.75">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="43.5">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="72.75">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="115.5">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>